<commit_message>
More references and updates
</commit_message>
<xml_diff>
--- a/data.TCGA/TCGA_cancers.xlsx
+++ b/data.TCGA/TCGA_cancers.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10312"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdozmorov/Documents/Work/VCU_work/misc/Zheng_Fu/TCGAsurvival/data.TCGA/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{779BF761-5463-CA4C-A057-A7323779ACF8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1080" windowWidth="25600" windowHeight="14980" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="1080" windowWidth="25600" windowHeight="14980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cancers" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>Cancer Name</t>
   </si>
@@ -247,12 +253,18 @@
   </si>
   <si>
     <t>UVM</t>
+  </si>
+  <si>
+    <t>STES</t>
+  </si>
+  <si>
+    <t>Stomach and esophageal cancer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -264,10 +276,12 @@
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -306,6 +320,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -630,17 +652,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="51" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -648,7 +672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -656,7 +680,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -664,7 +688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -672,7 +696,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -680,7 +704,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -688,7 +712,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -696,7 +720,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -704,7 +728,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -712,7 +736,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -720,7 +744,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -728,7 +752,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -736,7 +760,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1">
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -744,7 +768,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1">
+    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -752,7 +776,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1">
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
@@ -760,7 +784,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.75" customHeight="1">
+    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
@@ -768,7 +792,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1">
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
@@ -776,7 +800,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75" customHeight="1">
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
@@ -784,7 +808,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.75" customHeight="1">
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
@@ -792,7 +816,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75" customHeight="1">
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
@@ -800,7 +824,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.75" customHeight="1">
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
@@ -808,7 +832,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75" customHeight="1">
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>42</v>
       </c>
@@ -816,7 +840,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.75" customHeight="1">
+    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
@@ -824,7 +848,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75" customHeight="1">
+    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>46</v>
       </c>
@@ -832,7 +856,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75" customHeight="1">
+    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>48</v>
       </c>
@@ -840,7 +864,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.75" customHeight="1">
+    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>50</v>
       </c>
@@ -848,7 +872,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.75" customHeight="1">
+    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
         <v>52</v>
       </c>
@@ -856,7 +880,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.75" customHeight="1">
+    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
         <v>54</v>
       </c>
@@ -864,7 +888,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.75" customHeight="1">
+    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
         <v>56</v>
       </c>
@@ -872,7 +896,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.75" customHeight="1">
+    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>58</v>
       </c>
@@ -880,7 +904,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.75" customHeight="1">
+    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>60</v>
       </c>
@@ -888,7 +912,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.75" customHeight="1">
+    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>62</v>
       </c>
@@ -896,7 +920,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.75" customHeight="1">
+    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
         <v>64</v>
       </c>
@@ -904,7 +928,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15.75" customHeight="1">
+    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="2" t="s">
         <v>66</v>
       </c>
@@ -912,7 +936,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15.75" customHeight="1">
+    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
         <v>68</v>
       </c>
@@ -920,7 +944,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15.75" customHeight="1">
+    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
         <v>70</v>
       </c>
@@ -928,7 +952,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15.75" customHeight="1">
+    <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="2" t="s">
         <v>72</v>
       </c>
@@ -936,12 +960,20 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15.75" customHeight="1">
+    <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>